<commit_message>
updating protocol for part1b, finishing part1-b, updating part2 cleaning to reflect new template sturcture
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-7-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-7-occ-entry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7068ACFF-C4D1-364A-9CEA-EF6CE4F82AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E98308A-3A85-F248-8FE8-446AB9507F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15560" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2564,12 +2564,6 @@
     <t>idBy</t>
   </si>
   <si>
-    <t>assOcc</t>
-  </si>
-  <si>
-    <t>assTaxa</t>
-  </si>
-  <si>
     <t>vTaxonRank</t>
   </si>
   <si>
@@ -2895,6 +2889,12 @@
   </si>
   <si>
     <t>[conf]</t>
+  </si>
+  <si>
+    <t>assColl</t>
+  </si>
+  <si>
+    <t>assCollTaxa</t>
   </si>
 </sst>
 </file>
@@ -3385,10 +3385,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="116" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3430,43 +3430,43 @@
   <sheetData>
     <row r="1" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>3</v>
@@ -3478,10 +3478,10 @@
         <v>1</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>4</v>
@@ -3490,34 +3490,34 @@
         <v>5</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>6</v>
@@ -3537,37 +3537,37 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3">
         <v>19810528</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="U2"/>
       <c r="V2"/>
@@ -3585,34 +3585,34 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" s="3">
         <v>19810528</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U3"/>
       <c r="V3"/>
@@ -3629,34 +3629,34 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3">
         <v>19810528</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -3670,34 +3670,34 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3">
         <v>19810528</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF5"/>
     </row>
@@ -3712,34 +3712,34 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H6" s="3">
         <v>19810528</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF6"/>
     </row>
@@ -3754,34 +3754,34 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" s="3">
         <v>19810528</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -3795,34 +3795,34 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H8" s="3">
         <v>19810528</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF8"/>
     </row>
@@ -3837,34 +3837,34 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H9" s="3">
         <v>19810528</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF9"/>
     </row>
@@ -3879,34 +3879,34 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10" s="3">
         <v>19810528</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF10"/>
     </row>
@@ -3921,35 +3921,35 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H11" s="3">
         <v>19810528</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O11"/>
       <c r="P11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF11"/>
     </row>
@@ -3964,34 +3964,34 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H12" s="3">
         <v>19810528</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF12"/>
     </row>
@@ -4006,35 +4006,35 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H13" s="3">
         <v>19810528</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O13"/>
       <c r="P13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AB13"/>
       <c r="AC13"/>
@@ -4051,35 +4051,35 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H14" s="3">
         <v>19810528</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O14"/>
       <c r="P14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF14"/>
     </row>
@@ -4094,35 +4094,35 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3">
         <v>19810528</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O15"/>
       <c r="P15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF15"/>
     </row>
@@ -4137,35 +4137,35 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H16" s="3">
         <v>19810528</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O16"/>
       <c r="P16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF16"/>
     </row>
@@ -4180,35 +4180,35 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H17" s="3">
         <v>19810528</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O17"/>
       <c r="P17" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF17"/>
     </row>
@@ -4223,35 +4223,35 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H18" s="3">
         <v>19810528</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O18"/>
       <c r="P18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF18"/>
     </row>
@@ -4266,35 +4266,35 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H19" s="3">
         <v>19810528</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O19"/>
       <c r="P19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF19"/>
     </row>
@@ -4309,35 +4309,35 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H20" s="3">
         <v>19810528</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O20"/>
       <c r="P20" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF20"/>
     </row>
@@ -4352,35 +4352,35 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H21" s="3">
         <v>19810528</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O21"/>
       <c r="P21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF21"/>
     </row>
@@ -4395,35 +4395,35 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H22" s="3">
         <v>19810528</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O22"/>
       <c r="P22" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF22"/>
     </row>
@@ -4438,35 +4438,35 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H23" s="3">
         <v>19810528</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O23"/>
       <c r="P23" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AF23"/>
     </row>
@@ -4481,31 +4481,31 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H24" s="3">
         <v>19810528</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O24"/>
       <c r="AF24"/>
@@ -4521,31 +4521,31 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H25" s="3">
         <v>19810528</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O25"/>
       <c r="AF25"/>
@@ -4561,31 +4561,31 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H26" s="3">
         <v>19810528</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O26"/>
       <c r="AF26"/>
@@ -4601,31 +4601,31 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H27" s="3">
         <v>19810528</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P27"/>
       <c r="AF27"/>
@@ -4641,31 +4641,31 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H28" s="3">
         <v>19810528</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF28"/>
     </row>
@@ -4680,31 +4680,31 @@
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H29" s="3">
         <v>19810528</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF29"/>
     </row>
@@ -4719,31 +4719,31 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H30" s="3">
         <v>19810528</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF30"/>
     </row>
@@ -4758,34 +4758,34 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H31" s="3">
         <v>19810528</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -4799,31 +4799,31 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H32" s="3">
         <v>19810528</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -4837,31 +4837,31 @@
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H33" s="3">
         <v>19810528</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -4875,31 +4875,31 @@
         <v>11</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H34" s="3">
         <v>19810528</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -4913,31 +4913,31 @@
         <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H35" s="3">
         <v>19810528</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="34" x14ac:dyDescent="0.2">
@@ -4951,31 +4951,31 @@
         <v>13</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H36" s="3">
         <v>19810528</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -4992,16 +4992,16 @@
         <v>19810528</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5015,31 +5015,31 @@
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H38" s="3">
         <v>19810528</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5053,31 +5053,31 @@
         <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H39" s="3">
         <v>19810528</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5091,31 +5091,31 @@
         <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H40" s="3">
         <v>19810528</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5129,31 +5129,31 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H41" s="3">
         <v>19810528</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5167,31 +5167,31 @@
         <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42" s="3">
         <v>19810528</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5205,31 +5205,31 @@
         <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H43" s="3">
         <v>19810528</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5243,31 +5243,31 @@
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H44" s="3">
         <v>19810528</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5281,31 +5281,31 @@
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H45" s="3">
         <v>19810528</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5319,31 +5319,31 @@
         <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H46" s="3">
         <v>19810528</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5357,34 +5357,34 @@
         <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H47" s="3">
         <v>19810528</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF47" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5398,31 +5398,31 @@
         <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H48" s="3">
         <v>19810528</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5436,31 +5436,31 @@
         <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H49" s="3">
         <v>19810528</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5474,34 +5474,34 @@
         <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H50" s="3">
         <v>19810528</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF50" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5515,31 +5515,31 @@
         <v>28</v>
       </c>
       <c r="D51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H51" s="3">
         <v>19810528</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5553,31 +5553,31 @@
         <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H52" s="3">
         <v>19810528</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5591,31 +5591,31 @@
         <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H53" s="3">
         <v>19810528</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5629,31 +5629,31 @@
         <v>31</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E54" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="G54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H54" s="3">
         <v>19810528</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5667,31 +5667,31 @@
         <v>32</v>
       </c>
       <c r="D55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H55" s="3">
         <v>19810528</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5705,34 +5705,34 @@
         <v>33</v>
       </c>
       <c r="D56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H56" s="3">
         <v>19810528</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF56" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5746,31 +5746,31 @@
         <v>34</v>
       </c>
       <c r="D57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H57" s="3">
         <v>19810528</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5784,31 +5784,31 @@
         <v>35</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H58" s="3">
         <v>19810528</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5822,31 +5822,31 @@
         <v>36</v>
       </c>
       <c r="D59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H59" s="3">
         <v>19810528</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5860,31 +5860,31 @@
         <v>37</v>
       </c>
       <c r="D60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H60" s="3">
         <v>19810528</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5898,31 +5898,31 @@
         <v>38</v>
       </c>
       <c r="D61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H61" s="3">
         <v>19810528</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5936,34 +5936,34 @@
         <v>39</v>
       </c>
       <c r="D62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H62" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF62" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H62" s="3">
-        <v>19810528</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF62" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:32" ht="17" x14ac:dyDescent="0.2">
@@ -5977,34 +5977,34 @@
         <v>40</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H63" s="3">
         <v>19810528</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AF63" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding new folders for specimen data entry, and digitizing HJ7 occurrence data until page 8
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-7-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-7-occ-entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049CEAFF-D743-264E-80F4-E8CE97F46819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5C6853-6821-2745-810A-D941D2DC9911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -2475,7 +2475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="362">
   <si>
     <t>habitat</t>
   </si>
@@ -3183,6 +3183,384 @@
   </si>
   <si>
     <t xml:space="preserve">new species name not found in region </t>
+  </si>
+  <si>
+    <t>Cirsium arvense</t>
+  </si>
+  <si>
+    <t>Myosotis laxa</t>
+  </si>
+  <si>
+    <t>Myosotis cf. laxa</t>
+  </si>
+  <si>
+    <t>Rubus discolor</t>
+  </si>
+  <si>
+    <t>Rubus armeniacus</t>
+  </si>
+  <si>
+    <t>Veronica americana</t>
+  </si>
+  <si>
+    <t>Geum macrophyllum</t>
+  </si>
+  <si>
+    <t>Sherardia arvensis</t>
+  </si>
+  <si>
+    <t>Allium cernuum</t>
+  </si>
+  <si>
+    <t>Carex deweyana</t>
+  </si>
+  <si>
+    <t>Festuca subuliflora</t>
+  </si>
+  <si>
+    <t>Selaginella wallacei</t>
+  </si>
+  <si>
+    <t>Mimulus guttatus</t>
+  </si>
+  <si>
+    <t>Erythranthe guttata</t>
+  </si>
+  <si>
+    <t>Pityrogramma triangularis</t>
+  </si>
+  <si>
+    <t>Pentagramma triangularis</t>
+  </si>
+  <si>
+    <t>Mimulus alsinoides</t>
+  </si>
+  <si>
+    <t>Erythranthe alsinoides</t>
+  </si>
+  <si>
+    <t>Monotropa uniflora</t>
+  </si>
+  <si>
+    <t>Chimaphila umbellata</t>
+  </si>
+  <si>
+    <t>Carex lyngbyei</t>
+  </si>
+  <si>
+    <t>Arabis glabra</t>
+  </si>
+  <si>
+    <t>Pyrus fusca</t>
+  </si>
+  <si>
+    <t>Malus fusca</t>
+  </si>
+  <si>
+    <t>Hypericum anagalloides</t>
+  </si>
+  <si>
+    <t>Mentha arvensis</t>
+  </si>
+  <si>
+    <t>Mentha arvense</t>
+  </si>
+  <si>
+    <t>Urtica dioica</t>
+  </si>
+  <si>
+    <t>Alnus rubra</t>
+  </si>
+  <si>
+    <t>Stellaria crispa</t>
+  </si>
+  <si>
+    <t>Trifolium microcephalum</t>
+  </si>
+  <si>
+    <t>Lepidium virginicum</t>
+  </si>
+  <si>
+    <t>Taxus brevifolia</t>
+  </si>
+  <si>
+    <t>Eriophyllum lanatum</t>
+  </si>
+  <si>
+    <t>Sonchus asper</t>
+  </si>
+  <si>
+    <t>Clarkia amoena</t>
+  </si>
+  <si>
+    <t>Agoseris grandiflora</t>
+  </si>
+  <si>
+    <t>Hypochaeris glabra</t>
+  </si>
+  <si>
+    <t>Tsuga heterophylla</t>
+  </si>
+  <si>
+    <t>Trifolium oliganthum</t>
+  </si>
+  <si>
+    <t>Arctium minus</t>
+  </si>
+  <si>
+    <t>Rosa nutkana</t>
+  </si>
+  <si>
+    <t>Gnaphalium uliginosum</t>
+  </si>
+  <si>
+    <t>Oenothera sarmentosa</t>
+  </si>
+  <si>
+    <t>unable to decipher specific epithet</t>
+  </si>
+  <si>
+    <t>Lemna minor</t>
+  </si>
+  <si>
+    <t>Ranunculus aquariatum</t>
+  </si>
+  <si>
+    <t>Ranunculus aquatilis</t>
+  </si>
+  <si>
+    <t>Prunus emarginata</t>
+  </si>
+  <si>
+    <t>Adenocaulon bicolor</t>
+  </si>
+  <si>
+    <t>Satureja douglasii</t>
+  </si>
+  <si>
+    <t>Clinopodium douglasii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">originally recorded as Yerba buena, crossed out </t>
+  </si>
+  <si>
+    <t>Achlys triphylla</t>
+  </si>
+  <si>
+    <t>Populus tremuloides</t>
+  </si>
+  <si>
+    <t>Typha latifolia</t>
+  </si>
+  <si>
+    <t>Eleocharis palustris</t>
+  </si>
+  <si>
+    <t>originally recorded as Spike rush, crossed out</t>
+  </si>
+  <si>
+    <t>Veronica officinalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentilla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fen far west of lake </t>
+  </si>
+  <si>
+    <t>Ranunculus flammula</t>
+  </si>
+  <si>
+    <t>Campanula scouleri</t>
+  </si>
+  <si>
+    <t>Acer glabrum</t>
+  </si>
+  <si>
+    <t>Stellaria media</t>
+  </si>
+  <si>
+    <t>Myriophyllum</t>
+  </si>
+  <si>
+    <t>Myriophyllum cf. sp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Potentilla  cf. sp. </t>
+  </si>
+  <si>
+    <t>sp. Bracketed</t>
+  </si>
+  <si>
+    <t>Potamogeton natans</t>
+  </si>
+  <si>
+    <t>Cardamine pensylvanica</t>
+  </si>
+  <si>
+    <t>Berberis aquifolium</t>
+  </si>
+  <si>
+    <t>Lathyrus nevadensis</t>
+  </si>
+  <si>
+    <t>Ranunculus acris</t>
+  </si>
+  <si>
+    <t>Anthriscus scandicina</t>
+  </si>
+  <si>
+    <t>Anthriscus caucalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asterisk beside taxon name; originally Umbellifera? </t>
+  </si>
+  <si>
+    <t>Phleum pratense</t>
+  </si>
+  <si>
+    <t>Nuphar polysepala</t>
+  </si>
+  <si>
+    <t>Galium trifidum</t>
+  </si>
+  <si>
+    <t>Carex obnupta</t>
+  </si>
+  <si>
+    <t>Equisetum arvense</t>
+  </si>
+  <si>
+    <t>Veronica scutellata</t>
+  </si>
+  <si>
+    <t>Goodyera oblongifolia</t>
+  </si>
+  <si>
+    <t>Arenaria macrophylla</t>
+  </si>
+  <si>
+    <t>Moehringia macrophylla</t>
+  </si>
+  <si>
+    <t>Arabis hirsuta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very rare in area, maybe I did not decipher name right? </t>
+  </si>
+  <si>
+    <t>small island on east end of Prevost Island</t>
+  </si>
+  <si>
+    <t>Elymus mollis</t>
+  </si>
+  <si>
+    <t>Leymus mollis</t>
+  </si>
+  <si>
+    <t>Plectritis congesta</t>
+  </si>
+  <si>
+    <t>Sedum lanceolatum</t>
+  </si>
+  <si>
+    <t>Vicia americana</t>
+  </si>
+  <si>
+    <t>Camassia leichtlinii</t>
+  </si>
+  <si>
+    <t>Zygadenus venenosus</t>
+  </si>
+  <si>
+    <t>Toxicoscordion venenosum</t>
+  </si>
+  <si>
+    <t>on islands to south of Prevost Island</t>
+  </si>
+  <si>
+    <t>North East point of Prevost Island</t>
+  </si>
+  <si>
+    <t>cannot decipher genus name</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Lychnis coronaria</t>
+  </si>
+  <si>
+    <t>Silene coronaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spreading </t>
+  </si>
+  <si>
+    <t>Listera cordata</t>
+  </si>
+  <si>
+    <t>Neottia cordata</t>
+  </si>
+  <si>
+    <t>G. purpurea</t>
+  </si>
+  <si>
+    <t>[G] microcephala</t>
+  </si>
+  <si>
+    <t>[G] purpurea</t>
+  </si>
+  <si>
+    <t>around old light keepers house</t>
+  </si>
+  <si>
+    <t>Vinca major</t>
+  </si>
+  <si>
+    <t>persistant</t>
+  </si>
+  <si>
+    <t>qualitative</t>
+  </si>
+  <si>
+    <t>Sedum album</t>
+  </si>
+  <si>
+    <t>Santolina chamaecyparissus</t>
+  </si>
+  <si>
+    <t>Hypericum calycinum</t>
+  </si>
+  <si>
+    <t>varigated</t>
+  </si>
+  <si>
+    <t>Cytisus scoparius</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single at sea edge </t>
+  </si>
+  <si>
+    <t>Linum valerian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cannot decipher name it was replaced with </t>
+  </si>
+  <si>
+    <t>vegetative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-flowering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myriophyllum cf. sp. </t>
   </si>
 </sst>
 </file>
@@ -3359,10 +3737,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3684,12 +4062,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AF134"/>
+  <dimension ref="A1:AF222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
+      <selection pane="bottomLeft" activeCell="F224" sqref="F224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7442,6 +7820,9 @@
       <c r="A100" s="3">
         <v>4</v>
       </c>
+      <c r="B100" s="3">
+        <v>1</v>
+      </c>
       <c r="C100" s="3" t="s">
         <v>177</v>
       </c>
@@ -7456,6 +7837,21 @@
       </c>
       <c r="G100" s="3" t="s">
         <v>178</v>
+      </c>
+      <c r="H100" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L100" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="AB100" s="3" t="s">
         <v>185</v>
@@ -7465,6 +7861,9 @@
       <c r="A101" s="3">
         <v>4</v>
       </c>
+      <c r="B101" s="3">
+        <v>2</v>
+      </c>
       <c r="C101" s="3" t="s">
         <v>182</v>
       </c>
@@ -7480,11 +7879,32 @@
       <c r="G101" s="3" t="s">
         <v>183</v>
       </c>
+      <c r="H101" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L101" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB101" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="102" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
+        <v>4</v>
+      </c>
+      <c r="B102" s="3">
+        <v>3</v>
+      </c>
       <c r="C102" s="3" t="s">
         <v>187</v>
       </c>
@@ -7497,11 +7917,32 @@
       <c r="F102" s="3" t="s">
         <v>186</v>
       </c>
+      <c r="H102" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB102" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="103" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3">
+        <v>4</v>
+      </c>
+      <c r="B103" s="3">
+        <v>4</v>
+      </c>
       <c r="C103" s="3" t="s">
         <v>191</v>
       </c>
@@ -7514,8 +7955,29 @@
       <c r="F103" s="3" t="s">
         <v>191</v>
       </c>
+      <c r="H103" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="104" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="3">
+        <v>4</v>
+      </c>
+      <c r="B104" s="3">
+        <v>5</v>
+      </c>
       <c r="C104" s="3" t="s">
         <v>193</v>
       </c>
@@ -7528,11 +7990,32 @@
       <c r="F104" s="3" t="s">
         <v>192</v>
       </c>
+      <c r="H104" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB104" s="3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="105" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A105" s="3">
+        <v>4</v>
+      </c>
+      <c r="B105" s="3">
+        <v>6</v>
+      </c>
       <c r="C105" s="3" t="s">
         <v>189</v>
       </c>
@@ -7545,11 +8028,32 @@
       <c r="F105" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="H105" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L105" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB105" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="106" spans="1:32" ht="119" x14ac:dyDescent="0.2">
+      <c r="A106" s="3">
+        <v>4</v>
+      </c>
+      <c r="B106" s="3">
+        <v>7</v>
+      </c>
       <c r="C106" s="3" t="s">
         <v>196</v>
       </c>
@@ -7562,11 +8066,32 @@
       <c r="F106" s="3" t="s">
         <v>197</v>
       </c>
+      <c r="H106" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB106" s="3" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="107" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>4</v>
+      </c>
+      <c r="B107" s="3">
+        <v>8</v>
+      </c>
       <c r="C107" s="3" t="s">
         <v>199</v>
       </c>
@@ -7579,8 +8104,29 @@
       <c r="F107" s="3" t="s">
         <v>199</v>
       </c>
+      <c r="H107" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K107" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L107" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="108" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>4</v>
+      </c>
+      <c r="B108" s="3">
+        <v>9</v>
+      </c>
       <c r="C108" s="3" t="s">
         <v>200</v>
       </c>
@@ -7593,8 +8139,29 @@
       <c r="F108" s="3" t="s">
         <v>200</v>
       </c>
+      <c r="H108" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="109" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>4</v>
+      </c>
+      <c r="B109" s="3">
+        <v>10</v>
+      </c>
       <c r="C109" s="3" t="s">
         <v>201</v>
       </c>
@@ -7607,11 +8174,32 @@
       <c r="F109" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="H109" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J109" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K109" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L109" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AF109" s="3" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>4</v>
+      </c>
+      <c r="B110" s="3">
+        <v>11</v>
+      </c>
       <c r="C110" s="3" t="s">
         <v>203</v>
       </c>
@@ -7624,11 +8212,32 @@
       <c r="F110" s="3" t="s">
         <v>203</v>
       </c>
+      <c r="H110" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB110" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="111" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>4</v>
+      </c>
+      <c r="B111" s="3">
+        <v>12</v>
+      </c>
       <c r="C111" s="3" t="s">
         <v>204</v>
       </c>
@@ -7641,8 +8250,29 @@
       <c r="F111" s="3" t="s">
         <v>204</v>
       </c>
+      <c r="H111" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K111" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L111" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="112" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>4</v>
+      </c>
+      <c r="B112" s="3">
+        <v>13</v>
+      </c>
       <c r="C112" s="3" t="s">
         <v>205</v>
       </c>
@@ -7652,11 +8282,32 @@
       <c r="E112" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F112" s="9" t="s">
+      <c r="F112" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="113" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H112" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L112" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>4</v>
+      </c>
+      <c r="B113" s="3">
+        <v>14</v>
+      </c>
       <c r="C113" s="3" t="s">
         <v>206</v>
       </c>
@@ -7666,11 +8317,32 @@
       <c r="E113" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F113" s="9" t="s">
+      <c r="F113" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="114" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H113" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K113" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L113" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>4</v>
+      </c>
+      <c r="B114" s="3">
+        <v>15</v>
+      </c>
       <c r="C114" s="3" t="s">
         <v>207</v>
       </c>
@@ -7683,8 +8355,29 @@
       <c r="F114" s="3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="115" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H114" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>4</v>
+      </c>
+      <c r="B115" s="3">
+        <v>16</v>
+      </c>
       <c r="C115" s="3" t="s">
         <v>209</v>
       </c>
@@ -7697,8 +8390,29 @@
       <c r="F115" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="116" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H115" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K115" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L115" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>4</v>
+      </c>
+      <c r="B116" s="3">
+        <v>17</v>
+      </c>
       <c r="C116" s="3" t="s">
         <v>210</v>
       </c>
@@ -7711,8 +8425,29 @@
       <c r="F116" s="3" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="117" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="H116" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>4</v>
+      </c>
+      <c r="B117" s="3">
+        <v>18</v>
+      </c>
       <c r="C117" s="3" t="s">
         <v>211</v>
       </c>
@@ -7725,8 +8460,29 @@
       <c r="F117" s="3" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="118" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H117" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L117" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>4</v>
+      </c>
+      <c r="B118" s="3">
+        <v>19</v>
+      </c>
       <c r="C118" s="3" t="s">
         <v>180</v>
       </c>
@@ -7739,8 +8495,29 @@
       <c r="F118" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="119" spans="3:32" ht="102" x14ac:dyDescent="0.2">
+      <c r="H118" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L118" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:32" ht="102" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>4</v>
+      </c>
+      <c r="B119" s="3">
+        <v>20</v>
+      </c>
       <c r="C119" s="3" t="s">
         <v>181</v>
       </c>
@@ -7753,11 +8530,32 @@
       <c r="F119" s="3" t="s">
         <v>181</v>
       </c>
+      <c r="H119" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K119" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L119" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB119" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>4</v>
+      </c>
+      <c r="B120" s="3">
+        <v>21</v>
+      </c>
       <c r="C120" s="3" t="s">
         <v>213</v>
       </c>
@@ -7767,11 +8565,32 @@
       <c r="E120" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F120" s="10" t="s">
+      <c r="F120" s="9" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="121" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H120" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K120" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L120" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>4</v>
+      </c>
+      <c r="B121" s="3">
+        <v>22</v>
+      </c>
       <c r="C121" s="3" t="s">
         <v>215</v>
       </c>
@@ -7784,8 +8603,29 @@
       <c r="F121" s="3" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="122" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H121" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K121" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L121" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="122" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>4</v>
+      </c>
+      <c r="B122" s="3">
+        <v>23</v>
+      </c>
       <c r="C122" s="3" t="s">
         <v>216</v>
       </c>
@@ -7798,8 +8638,29 @@
       <c r="F122" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="123" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H122" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K122" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L122" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>4</v>
+      </c>
+      <c r="B123" s="3">
+        <v>24</v>
+      </c>
       <c r="C123" s="3" t="s">
         <v>217</v>
       </c>
@@ -7809,19 +8670,76 @@
       <c r="E123" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F123" s="9" t="s">
+      <c r="F123" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="124" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H123" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K123" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L123" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>4</v>
+      </c>
+      <c r="B124" s="3">
+        <v>25</v>
+      </c>
+      <c r="H124" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L124" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AF124" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="125" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>4</v>
+      </c>
+      <c r="B125" s="3">
+        <v>26</v>
+      </c>
       <c r="C125" s="3" t="s">
         <v>219</v>
       </c>
+      <c r="H125" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K125" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L125" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="O125" s="3" t="s">
         <v>220</v>
       </c>
@@ -7829,7 +8747,13 @@
         <v>221</v>
       </c>
     </row>
-    <row r="126" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>4</v>
+      </c>
+      <c r="B126" s="3">
+        <v>27</v>
+      </c>
       <c r="C126" s="3" t="s">
         <v>222</v>
       </c>
@@ -7842,8 +8766,29 @@
       <c r="F126" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="127" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="H126" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L126" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="127" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>4</v>
+      </c>
+      <c r="B127" s="3">
+        <v>28</v>
+      </c>
       <c r="C127" s="3" t="s">
         <v>223</v>
       </c>
@@ -7856,11 +8801,32 @@
       <c r="F127" s="3" t="s">
         <v>223</v>
       </c>
+      <c r="H127" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J127" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K127" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L127" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB127" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="128" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>4</v>
+      </c>
+      <c r="B128" s="3">
+        <v>29</v>
+      </c>
       <c r="C128" s="3" t="s">
         <v>224</v>
       </c>
@@ -7873,8 +8839,29 @@
       <c r="F128" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="129" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H128" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L128" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>4</v>
+      </c>
+      <c r="B129" s="3">
+        <v>30</v>
+      </c>
       <c r="C129" s="3" t="s">
         <v>226</v>
       </c>
@@ -7887,16 +8874,58 @@
       <c r="F129" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="130" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H129" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K129" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L129" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="130" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>4</v>
+      </c>
+      <c r="B130" s="3">
+        <v>31</v>
+      </c>
       <c r="C130" s="3" t="s">
         <v>227</v>
       </c>
+      <c r="H130" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L130" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AF130" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="131" spans="3:32" ht="51" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>4</v>
+      </c>
+      <c r="B131" s="3">
+        <v>32</v>
+      </c>
       <c r="C131" s="3" t="s">
         <v>229</v>
       </c>
@@ -7909,11 +8938,32 @@
       <c r="F131" s="3" t="s">
         <v>229</v>
       </c>
+      <c r="H131" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K131" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L131" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AB131" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>4</v>
+      </c>
+      <c r="B132" s="3">
+        <v>33</v>
+      </c>
       <c r="C132" s="3" t="s">
         <v>231</v>
       </c>
@@ -7926,8 +8976,29 @@
       <c r="F132" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="133" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H132" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>4</v>
+      </c>
+      <c r="B133" s="3">
+        <v>34</v>
+      </c>
       <c r="C133" s="3" t="s">
         <v>232</v>
       </c>
@@ -7940,8 +9011,29 @@
       <c r="F133" s="3" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="134" spans="3:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="H133" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L133" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>4</v>
+      </c>
+      <c r="B134" s="3">
+        <v>35</v>
+      </c>
       <c r="C134" s="3" t="s">
         <v>233</v>
       </c>
@@ -7954,8 +9046,3082 @@
       <c r="F134" s="3" t="s">
         <v>234</v>
       </c>
+      <c r="H134" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="AF134" s="3" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="135" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>5</v>
+      </c>
+      <c r="B135" s="3">
+        <v>1</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H135" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J135" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L135" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="136" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>5</v>
+      </c>
+      <c r="B136" s="3">
+        <v>2</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H136" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB136" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="137" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>5</v>
+      </c>
+      <c r="B137" s="3">
+        <v>3</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H137" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J137" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K137" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L137" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="138" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>5</v>
+      </c>
+      <c r="B138" s="3">
+        <v>4</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H138" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="139" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>5</v>
+      </c>
+      <c r="B139" s="3">
+        <v>5</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H139" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J139" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K139" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L139" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>5</v>
+      </c>
+      <c r="B140" s="3">
+        <v>6</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H140" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L140" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>5</v>
+      </c>
+      <c r="B141" s="3">
+        <v>7</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H141" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L141" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="142" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>5</v>
+      </c>
+      <c r="B142" s="3">
+        <v>8</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H142" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L142" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="143" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>5</v>
+      </c>
+      <c r="B143" s="3">
+        <v>9</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H143" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J143" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L143" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="144" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>5</v>
+      </c>
+      <c r="B144" s="3">
+        <v>10</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H144" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L144" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>5</v>
+      </c>
+      <c r="B145" s="3">
+        <v>11</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H145" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J145" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L145" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>5</v>
+      </c>
+      <c r="B146" s="3">
+        <v>12</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H146" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K146" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L146" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>5</v>
+      </c>
+      <c r="B147" s="3">
+        <v>13</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H147" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>5</v>
+      </c>
+      <c r="B148" s="3">
+        <v>14</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H148" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>5</v>
+      </c>
+      <c r="B149" s="3">
+        <v>15</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H149" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L149" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>5</v>
+      </c>
+      <c r="B150" s="3">
+        <v>16</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H150" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L150" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>5</v>
+      </c>
+      <c r="B151" s="3">
+        <v>17</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H151" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L151" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>5</v>
+      </c>
+      <c r="B152" s="3">
+        <v>18</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H152" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L152" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>5</v>
+      </c>
+      <c r="B153" s="3">
+        <v>19</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H153" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L153" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>5</v>
+      </c>
+      <c r="B154" s="3">
+        <v>20</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H154" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L154" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>5</v>
+      </c>
+      <c r="B155" s="3">
+        <v>21</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H155" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L155" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>5</v>
+      </c>
+      <c r="B156" s="3">
+        <v>22</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H156" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L156" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>5</v>
+      </c>
+      <c r="B157" s="3">
+        <v>23</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H157" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J157" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L157" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>5</v>
+      </c>
+      <c r="B158" s="3">
+        <v>24</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H158" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L158" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>5</v>
+      </c>
+      <c r="B159" s="3">
+        <v>25</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H159" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J159" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K159" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L159" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>5</v>
+      </c>
+      <c r="B160" s="3">
+        <v>26</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="H160" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I160" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J160" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K160" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L160" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="161" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>5</v>
+      </c>
+      <c r="B161" s="3">
+        <v>27</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H161" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K161" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L161" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="162" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>5</v>
+      </c>
+      <c r="B162" s="3">
+        <v>28</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H162" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I162" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J162" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K162" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L162" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>5</v>
+      </c>
+      <c r="B163" s="3">
+        <v>29</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H163" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I163" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J163" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K163" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L163" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>5</v>
+      </c>
+      <c r="B164" s="3">
+        <v>30</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H164" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L164" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>5</v>
+      </c>
+      <c r="B165" s="3">
+        <v>31</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H165" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J165" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K165" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L165" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="166" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>5</v>
+      </c>
+      <c r="B166" s="3">
+        <v>32</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H166" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J166" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K166" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L166" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="167" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>5</v>
+      </c>
+      <c r="B167" s="3">
+        <v>33</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H167" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I167" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J167" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K167" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L167" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="168" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A168" s="3">
+        <v>5</v>
+      </c>
+      <c r="B168" s="3">
+        <v>34</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H168" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I168" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J168" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K168" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L168" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="169" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A169" s="3">
+        <v>5</v>
+      </c>
+      <c r="B169" s="3">
+        <v>35</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H169" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I169" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J169" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K169" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L169" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="170" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>5</v>
+      </c>
+      <c r="B170" s="3">
+        <v>36</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H170" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J170" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K170" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L170" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="171" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A171" s="3">
+        <v>6</v>
+      </c>
+      <c r="B171" s="3">
+        <v>1</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H171" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I171" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J171" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K171" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L171" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="172" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>6</v>
+      </c>
+      <c r="B172" s="3">
+        <v>2</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H172" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K172" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L172" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="173" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A173" s="3">
+        <v>6</v>
+      </c>
+      <c r="B173" s="3">
+        <v>3</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H173" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J173" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K173" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L173" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF173" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="174" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
+        <v>6</v>
+      </c>
+      <c r="B174" s="3">
+        <v>4</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H174" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J174" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K174" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L174" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A175" s="3">
+        <v>6</v>
+      </c>
+      <c r="B175" s="3">
+        <v>5</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H175" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I175" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J175" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K175" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L175" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="176" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
+        <v>6</v>
+      </c>
+      <c r="B176" s="3">
+        <v>6</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H176" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J176" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K176" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L176" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="177" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>6</v>
+      </c>
+      <c r="B177" s="3">
+        <v>7</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="H177" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I177" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J177" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K177" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L177" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="178" spans="1:28" ht="68" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>6</v>
+      </c>
+      <c r="B178" s="3">
+        <v>8</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="H178" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J178" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K178" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L178" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB178" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="179" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>6</v>
+      </c>
+      <c r="B179" s="3">
+        <v>9</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H179" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I179" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K179" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L179" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="180" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>6</v>
+      </c>
+      <c r="B180" s="3">
+        <v>10</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="H180" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J180" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K180" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L180" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="181" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
+        <v>6</v>
+      </c>
+      <c r="B181" s="3">
+        <v>11</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H181" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I181" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J181" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K181" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L181" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="182" spans="1:28" ht="68" x14ac:dyDescent="0.2">
+      <c r="A182" s="3">
+        <v>6</v>
+      </c>
+      <c r="B182" s="3">
+        <v>12</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H182" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I182" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J182" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K182" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L182" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB182" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="183" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A183" s="3">
+        <v>6</v>
+      </c>
+      <c r="B183" s="3">
+        <v>13</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H183" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I183" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J183" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K183" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L183" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="184" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+      <c r="A184" s="3">
+        <v>6</v>
+      </c>
+      <c r="B184" s="3">
+        <v>14</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="H184" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I184" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J184" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K184" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L184" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O184" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="P184" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="185" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A185" s="3">
+        <v>6</v>
+      </c>
+      <c r="B185" s="3">
+        <v>15</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H185" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I185" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J185" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K185" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L185" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="186" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>6</v>
+      </c>
+      <c r="B186" s="3">
+        <v>16</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H186" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I186" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J186" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K186" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L186" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="187" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
+        <v>6</v>
+      </c>
+      <c r="B187" s="3">
+        <v>17</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H187" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I187" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J187" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K187" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L187" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="188" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A188" s="3">
+        <v>6</v>
+      </c>
+      <c r="B188" s="3">
+        <v>18</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H188" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I188" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J188" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K188" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L188" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="189" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A189" s="3">
+        <v>6</v>
+      </c>
+      <c r="B189" s="3">
+        <v>19</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H189" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I189" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J189" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K189" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L189" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="190" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
+        <v>6</v>
+      </c>
+      <c r="B190" s="3">
+        <v>20</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H190" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I190" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J190" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K190" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L190" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB190" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="191" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
+        <v>6</v>
+      </c>
+      <c r="B191" s="3">
+        <v>21</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H191" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I191" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J191" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K191" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L191" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="192" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="A192" s="3">
+        <v>6</v>
+      </c>
+      <c r="B192" s="3">
+        <v>22</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="H192" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I192" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J192" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K192" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L192" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A193" s="3">
+        <v>6</v>
+      </c>
+      <c r="B193" s="3">
+        <v>23</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="H193" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I193" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J193" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K193" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L193" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="194" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A194" s="3">
+        <v>6</v>
+      </c>
+      <c r="B194" s="3">
+        <v>24</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H194" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I194" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J194" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K194" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L194" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="195" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A195" s="3">
+        <v>6</v>
+      </c>
+      <c r="B195" s="3">
+        <v>25</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H195" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I195" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J195" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K195" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L195" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="196" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A196" s="3">
+        <v>6</v>
+      </c>
+      <c r="B196" s="3">
+        <v>26</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H196" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I196" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J196" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K196" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L196" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB196" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="197" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A197" s="3">
+        <v>6</v>
+      </c>
+      <c r="B197" s="3">
+        <v>27</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H197" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I197" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J197" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K197" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L197" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="198" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A198" s="3">
+        <v>6</v>
+      </c>
+      <c r="B198" s="3">
+        <v>28</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F198" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H198" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I198" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J198" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K198" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L198" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="199" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A199" s="3">
+        <v>6</v>
+      </c>
+      <c r="B199" s="3">
+        <v>29</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F199" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H199" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I199" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J199" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K199" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L199" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="200" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A200" s="3">
+        <v>6</v>
+      </c>
+      <c r="B200" s="3">
+        <v>30</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="H200" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I200" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J200" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K200" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L200" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="201" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A201" s="3">
+        <v>6</v>
+      </c>
+      <c r="B201" s="3">
+        <v>31</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H201" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I201" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J201" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K201" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L201" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="202" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A202" s="3">
+        <v>6</v>
+      </c>
+      <c r="B202" s="3">
+        <v>32</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H202" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I202" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J202" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K202" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L202" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="203" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A203" s="3">
+        <v>6</v>
+      </c>
+      <c r="B203" s="3">
+        <v>33</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H203" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I203" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J203" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K203" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L203" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="204" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A204" s="3">
+        <v>6</v>
+      </c>
+      <c r="B204" s="3">
+        <v>34</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H204" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I204" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J204" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K204" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L204" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="205" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A205" s="3">
+        <v>6</v>
+      </c>
+      <c r="B205" s="3">
+        <v>35</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="H205" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I205" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J205" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K205" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L205" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF205" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="206" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A206" s="3">
+        <v>7</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="H206" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I206" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J206" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K206" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L206" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="207" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C207" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H207" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I207" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J207" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K207" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L207" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="208" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C208" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H208" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I208" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J208" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K208" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L208" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="209" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C209" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F209" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="H209" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I209" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J209" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K209" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L209" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="210" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C210" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H210" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I210" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J210" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K210" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L210" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="211" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C211" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F211" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H211" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="J211" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K211" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L211" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C212" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="H212" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J212" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K212" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L212" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF212" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="213" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C213" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H213" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J213" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K213" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L213" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB213" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="214" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C214" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H214" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I214" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J214" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K214" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L214" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF214" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="215" spans="3:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="C215" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F215" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="H215" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I215" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J215" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K215" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L215" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="216" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C216" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H216" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I216" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J216" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K216" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L216" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P216" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z216" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AA216" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="AB216" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="217" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C217" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F217" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H217" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I217" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J217" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K217" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L217" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P217" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z217" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AA217" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="218" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C218" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F218" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="H218" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I218" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J218" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K218" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L218" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P218" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z218" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AA218" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="219" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C219" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F219" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H219" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I219" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J219" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K219" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L219" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P219" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z219" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AA219" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="220" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C220" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F220" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H220" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I220" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J220" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K220" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L220" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P220" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z220" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA220" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB220" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="221" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C221" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="H221" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I221" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J221" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K221" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L221" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P221" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB221" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="AC221" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="AF221" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="222" spans="3:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="C222" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="H222" s="3">
+        <v>19810528</v>
+      </c>
+      <c r="I222" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J222" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K222" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L222" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P222" s="3" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>